<commit_message>
Only need to do a testrun now
</commit_message>
<xml_diff>
--- a/CANumbers.xlsx
+++ b/CANumbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CANumbers" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">CA Number</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">NOTE : Only add CA Number, other fields will be autofilled.</t>
   </si>
   <si>
+    <t xml:space="preserve">Mr. RAMESHWAR DASS BOHET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLOT NO 19 KH. NO. 38/22 GROUND FLOOR GRAM SABHA STREET NO. GALI NO-2 VILLAGE MAMURPUR CITY DELHI 110040 LANDMARK NEAR RADHA SWAMI ASHRAM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Don’t change the name of file or worksheets.</t>
   </si>
   <si>
@@ -52,24 +58,25 @@
     <t xml:space="preserve">Complaint Number</t>
   </si>
   <si>
-    <t xml:space="preserve">No supply in area since 1 hour.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is no electricity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electricity is affected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No supply, get it fixed immediately.</t>
+    <t xml:space="preserve">some complaint number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No supply in area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No electricity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power breakdown in area, get it fixed immedieately.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD\ H:MM:SS"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -150,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,7 +174,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,21 +205,23 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="49.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="146.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="6" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="44.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -232,6 +249,12 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>60014463164</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -241,9 +264,6 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>60020461996</v>
-      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -252,9 +272,7 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>60019216229</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -264,7 +282,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -294,27 +312,49 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>43677.0261515908</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>60014463164</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>43677.0271245861</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>60014463164</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -334,36 +374,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="42.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="4" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -371,8 +406,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -390,15 +425,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="4" width="11.52"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>